<commit_message>
Agregada funcionalidad de logout
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Desktop\Entornos\App_notas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FB2C83-82A4-4797-9AC4-13EEBC1FE307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2AD42C-2380-4D73-AA5F-003A76C7E3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14610" yWindow="1905" windowWidth="22065" windowHeight="17700" xr2:uid="{2126B46F-AB51-420E-A56F-A17DE3375258}"/>
   </bookViews>
@@ -442,7 +442,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Correcion entrada index entero
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Desktop\Entornos\App_notas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2AD42C-2380-4D73-AA5F-003A76C7E3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129F09C6-E982-47C7-B164-DFA32074E21F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14610" yWindow="1905" windowWidth="22065" windowHeight="17700" xr2:uid="{2126B46F-AB51-420E-A56F-A17DE3375258}"/>
   </bookViews>
@@ -47,13 +47,13 @@
     <t>María</t>
   </si>
   <si>
-    <t>HomeWork 1</t>
-  </si>
-  <si>
     <t>Exposicion</t>
   </si>
   <si>
     <t>Quiz</t>
+  </si>
+  <si>
+    <t>HomeWork_1</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,13 +455,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>